<commit_message>
20180802 - Fin de Contrato
Repositorio de Mineria de datos al 30 de septiembre de 2018.
</commit_message>
<xml_diff>
--- a/02_Aire/P0218/P0218_PM10.xlsx
+++ b/02_Aire/P0218/P0218_PM10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PCCS\01_Dmine\02_Aire\P0218\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8EF66A73-88DD-4DF6-A7EF-66774BB95143}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C7F3FE4A-C79A-4847-B2E0-98BD683D26C8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4741,8 +4741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>